<commit_message>
Add key word extraction.
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="300 embedding" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="10">
   <si>
     <t>1, 2</t>
   </si>
@@ -967,10 +967,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,6 +1065,14 @@
       </c>
       <c r="E5" s="2">
         <v>0.4289</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0.35699999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -1178,7 +1186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
First version of my thesis.
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="300 embedding" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,8 @@
     <sheet name="100 embedding" sheetId="3" r:id="rId3"/>
     <sheet name="100 embedding by char" sheetId="6" r:id="rId4"/>
     <sheet name="Binary" sheetId="4" r:id="rId5"/>
-    <sheet name="Double Channel" sheetId="5" r:id="rId6"/>
+    <sheet name="Binary by char" sheetId="7" r:id="rId6"/>
+    <sheet name="Double Channel" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="13">
   <si>
     <t>1, 2</t>
   </si>
@@ -60,6 +61,9 @@
   </si>
   <si>
     <t>lstm</t>
+  </si>
+  <si>
+    <t>two_channel</t>
   </si>
 </sst>
 </file>
@@ -973,10 +977,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1082,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.35699999999999998</v>
+        <v>38.700000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1087,6 +1091,14 @@
       </c>
       <c r="B13">
         <v>44.86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>43.29</v>
       </c>
     </row>
   </sheetData>
@@ -1100,7 +1112,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="E5" sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,7 +1301,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="5">
-        <v>0.7671</v>
+        <v>0.78310000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1306,6 +1318,107 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.70069999999999999</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.77890000000000004</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.75109999999999999</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.74529999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.78120000000000001</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.79859999999999998</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.77990000000000004</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.7974</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.79590000000000005</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.79859999999999998</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.79279999999999995</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.80469999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.79730000000000001</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.80330000000000001</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.78410000000000002</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.80259999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Second version of my thesis.
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="300 embedding" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="14">
   <si>
     <t>1, 2</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>two_channel</t>
+  </si>
+  <si>
+    <t>two channel</t>
   </si>
 </sst>
 </file>
@@ -979,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,7 +1093,7 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>44.86</v>
+        <v>44.02</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1210,10 +1213,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,7 +1312,15 @@
         <v>11</v>
       </c>
       <c r="B17">
-        <v>81.77</v>
+        <v>81.96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>81.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some changes in my thesis.
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="300 embedding" sheetId="1" r:id="rId1"/>
@@ -988,7 +988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1090,8 +1090,8 @@
       <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9">
-        <v>41.54</v>
+      <c r="B9" s="5">
+        <v>0.38700000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1137,7 +1137,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="A1:E5"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,7 +1237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>